<commit_message>
Tambah TC002-001 buat test kawalpemilu dan benerin document summary
</commit_message>
<xml_diff>
--- a/Excel/Global_Report.xlsx
+++ b/Excel/Global_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Selenium_2024\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD21A2B-4463-4959-B72B-8C0D377E5222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7536A259-9F6B-459F-90AD-62E34B47D7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F15E9A0-1C50-4655-9A11-8F4BEDD34A56}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>122.0.1</t>
   </si>
   <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
     <t>Automation Team</t>
   </si>
   <si>
@@ -138,10 +135,13 @@
     <t>Yusuf Tri Wibowo</t>
   </si>
   <si>
-    <t>Google - Regression Test</t>
-  </si>
-  <si>
     <t>CR / IR / MR</t>
+  </si>
+  <si>
+    <t>https://kawalpemilu.org/</t>
+  </si>
+  <si>
+    <t>Kawal Pemilu - Regression Test</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B696D2-CFC8-42C4-915F-2368366EE231}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     <col min="8" max="8" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -626,37 +626,37 @@
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>